<commit_message>
Doc Présentation + suivi
</commit_message>
<xml_diff>
--- a/Doc/Suivi/Avancement taches.xlsx
+++ b/Doc/Suivi/Avancement taches.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="300" windowWidth="15600" windowHeight="11700"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
   <si>
     <t>Suivi de projet</t>
   </si>
@@ -151,13 +151,19 @@
   </si>
   <si>
     <t>Moyen</t>
+  </si>
+  <si>
+    <t>Risque</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,12 +289,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -361,6 +380,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -395,6 +415,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -570,28 +591,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
@@ -604,8 +625,11 @@
       <c r="D3" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="18.75">
+      <c r="E3" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
@@ -618,11 +642,15 @@
       <c r="D4" s="8">
         <v>3</v>
       </c>
+      <c r="E4" s="10">
+        <f>SUM(D4:D5)/2</f>
+        <v>2</v>
+      </c>
       <c r="F4" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -642,7 +670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="2" t="s">
         <v>44</v>
       </c>
@@ -650,7 +678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75">
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
@@ -661,7 +689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -674,8 +702,12 @@
       <c r="D8" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="E8" s="10">
+        <f>SUM(D8:D9)/2</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -689,12 +721,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75">
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -707,8 +739,12 @@
       <c r="D12" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="E12" s="11">
+        <f>SUM(D12:D18)/7</f>
+        <v>2.5714285714285716</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -722,7 +758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
@@ -736,7 +772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
@@ -750,7 +786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>11</v>
       </c>
@@ -764,7 +800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>35</v>
       </c>
@@ -778,7 +814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>21</v>
       </c>
@@ -792,12 +828,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18.75">
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
@@ -810,8 +846,12 @@
       <c r="D21" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="10">
+        <f>SUM(D21:D29)/9</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>14</v>
       </c>
@@ -825,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
@@ -839,7 +879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>16</v>
       </c>
@@ -853,7 +893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>17</v>
       </c>
@@ -867,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>18</v>
       </c>
@@ -881,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>19</v>
       </c>
@@ -895,7 +935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>20</v>
       </c>
@@ -909,7 +949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>36</v>
       </c>
@@ -923,12 +963,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18.75">
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>38</v>
       </c>
@@ -942,7 +982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>39</v>
       </c>
@@ -956,7 +996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>40</v>
       </c>
@@ -970,12 +1010,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18.75">
+    <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>30</v>
       </c>
@@ -988,8 +1028,12 @@
       <c r="D38" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="10">
+        <f>SUM(D38:D42)/5</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -1003,7 +1047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
@@ -1017,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
@@ -1031,7 +1075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>34</v>
       </c>
@@ -1052,12 +1096,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1065,12 +1109,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>